<commit_message>
trying to fix seemingly corrupt workbook
</commit_message>
<xml_diff>
--- a/random_wc_model_generator/data/fixtures/model_core.xlsx
+++ b/random_wc_model_generator/data/fixtures/model_core.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" state="visible" r:id="rId2"/>
@@ -35,16 +35,38 @@
     <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Submodels!$A$1:$I$5</definedName>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Taxon!$A$1:$B$6</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Model!$A$1:$B$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Model!$A$1:$B$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Model!$A$1:$B$5</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Taxon!$A$1:$B$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">Taxon!$A$1:$B$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Taxon!$A$1:$B$6</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Submodels!$A$1:$I$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">Submodels!$A$1:$I$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Submodels!$A$1:$I$5</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Species types'!$A$1:$J$84</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Species types'!$A$1:$J$84</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Species types'!$A$1:$J$84</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">Concentrations!$A$1:$D$66</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0" vbProcedure="false">Concentrations!$A$1:$D$66</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Concentrations!$A$1:$D$66</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase" vbProcedure="false">Reactions!$A$1:$I$87</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0" vbProcedure="false">Reactions!$A$1:$I$87</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Reactions!$A$1:$I$87</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase" vbProcedure="false">'Rate laws'!$A$1:$G$29</definedName>
+    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Rate laws'!$A$1:$G$29</definedName>
+    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Rate laws'!$A$1:$G$29</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$H$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$H$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Parameters!$A$1:$H$6</definedName>
     <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$R$20</definedName>
+    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0" vbProcedure="false">References!$A$1:$R$20</definedName>
+    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">References!$A$1:$R$20</definedName>
     <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase" vbProcedure="false">'Cross references'!$A$1:$I$20</definedName>
+    <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Cross references'!$A$1:$I$99</definedName>
+    <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Cross references'!$A$1:$I$20</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -3665,7 +3687,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="22">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3689,10 +3711,6 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3771,19 +3789,19 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3792,15 +3810,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Normal 2" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Normal 3" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -3916,14 +3933,16 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="E27:E29 B1"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="B4" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topRight" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.8178137651822"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.8137651821862"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="10.8178137651822"/>
   </cols>
   <sheetData>
@@ -3985,14 +4004,18 @@
   </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="E27:E29 B2"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="17.1376518218624"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="3" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="17.3522267206478"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="3" width="23.4574898785425"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="3" width="10.8178137651822"/>
   </cols>
   <sheetData>
@@ -4050,19 +4073,19 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" activeCellId="1" sqref="E27:E29 B2"/>
+      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="20.246963562753"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="22" width="28.2793522267206"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="12.2105263157895"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="22" width="28.7085020242915"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="12.4251012145749"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="3" width="8.1417004048583"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="18.5303643724696"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="22" width="32.8866396761134"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="3" width="16.1740890688259"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="22" width="33.4210526315789"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="3" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="3" width="10.8178137651822"/>
   </cols>
   <sheetData>
@@ -4231,13 +4254,13 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" activeCellId="1" sqref="E27:E29 B2"/>
+      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="3" min="1" style="3" width="10.8178137651822"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="32.9919028340081"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="33.5263157894737"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="3" width="10.8178137651822"/>
   </cols>
   <sheetData>
@@ -5020,20 +5043,20 @@
   </sheetPr>
   <dimension ref="A1:I99"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C58" activePane="bottomRight" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A58" activeCellId="0" sqref="A58"/>
-      <selection pane="bottomRight" activeCell="C58" activeCellId="1" sqref="E27:E29 C58"/>
+      <selection pane="bottomLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+      <selection pane="bottomRight" activeCell="I40" activeCellId="0" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="3" width="10.8178137651822"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="27.6356275303644"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="28.0647773279352"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="3" width="10.8178137651822"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="26.8866396761134"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="27.3157894736842"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="3" width="10.8178137651822"/>
   </cols>
   <sheetData>
@@ -5427,1348 +5450,1664 @@
         <v>970</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="1" t="s">
         <v>1020</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="2" t="s">
         <v>1021</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="3" t="s">
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="1" t="s">
         <v>1022</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="2" t="s">
         <v>1023</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G22" s="3" t="s">
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3" t="s">
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="1" t="s">
         <v>1024</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="2" t="s">
         <v>1025</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G23" s="3" t="s">
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="3" t="s">
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
         <v>1026</v>
       </c>
-      <c r="B24" s="3" t="n">
+      <c r="B24" s="1" t="n">
         <v>6197512</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="2" t="s">
         <v>1027</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G24" s="3" t="s">
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3" t="s">
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="1" t="s">
         <v>1028</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="2" t="s">
         <v>1029</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="3" t="s">
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="1" t="s">
         <v>1030</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="2" t="s">
         <v>1031</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G26" s="3" t="s">
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="3" t="s">
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
         <v>1026</v>
       </c>
-      <c r="B27" s="3" t="n">
+      <c r="B27" s="1" t="n">
         <v>77638054</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="2" t="s">
         <v>1032</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G27" s="3" t="s">
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="28" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="3" t="s">
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="1" t="s">
         <v>1033</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="2" t="s">
         <v>1034</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G28" s="3" t="s">
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="29" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="3" t="s">
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
         <v>1026</v>
       </c>
-      <c r="B29" s="3" t="n">
+      <c r="B29" s="1" t="n">
         <v>28724627</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="2" t="s">
         <v>1035</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G29" s="3" t="s">
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="30" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="3" t="s">
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="1" t="s">
         <v>1036</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="2" t="s">
         <v>1037</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G30" s="3" t="s">
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="31" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="3" t="s">
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
         <v>1026</v>
       </c>
-      <c r="B31" s="3" t="n">
+      <c r="B31" s="1" t="n">
         <v>10306892</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="2" t="s">
         <v>1038</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G31" s="3" t="s">
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="32" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="3" t="s">
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="1" t="s">
         <v>1039</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="2" t="s">
         <v>1040</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G32" s="3" t="s">
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="33" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="3" t="s">
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="1" t="s">
         <v>1041</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="2" t="s">
         <v>1042</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G33" s="3" t="s">
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="34" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="3" t="s">
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="1" t="s">
         <v>1043</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="2" t="s">
         <v>1044</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G34" s="3" t="s">
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="35" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="3" t="s">
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="1" t="s">
         <v>1045</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="2" t="s">
         <v>1046</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G35" s="3" t="s">
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="36" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="3" t="s">
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="1" t="s">
         <v>1047</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" s="2" t="s">
         <v>1048</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G36" s="3" t="s">
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="37" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="3" t="s">
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="1" t="s">
         <v>1049</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="2" t="s">
         <v>1050</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G37" s="3" t="s">
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="38" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="3" t="s">
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
         <v>1026</v>
       </c>
-      <c r="B38" s="3" t="n">
+      <c r="B38" s="1" t="n">
         <v>10251455</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C38" s="2" t="s">
         <v>1051</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G38" s="3" t="s">
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="39" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="3" t="s">
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="1" t="s">
         <v>1052</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C39" s="2" t="s">
         <v>1053</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G39" s="3" t="s">
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="40" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="3" t="s">
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="1" t="s">
         <v>1054</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C40" s="2" t="s">
         <v>1055</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G40" s="3" t="s">
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="41" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="3" t="s">
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="1" t="s">
         <v>1056</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C41" s="2" t="s">
         <v>1057</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G41" s="3" t="s">
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="42" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="3" t="s">
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="1" t="s">
         <v>1058</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C42" s="2" t="s">
         <v>1059</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G42" s="3" t="s">
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="43" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="3" t="s">
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="1" t="s">
         <v>1060</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C43" s="2" t="s">
         <v>1061</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G43" s="3" t="s">
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="44" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="3" t="s">
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+    </row>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="1" t="s">
         <v>1062</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C44" s="2" t="s">
         <v>1063</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G44" s="3" t="s">
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="45" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="3" t="s">
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="1" t="s">
         <v>1064</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C45" s="2" t="s">
         <v>1065</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G45" s="3" t="s">
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="46" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="3" t="s">
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+    </row>
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B46" s="1" t="s">
         <v>1066</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C46" s="2" t="s">
         <v>1067</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G46" s="3" t="s">
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="47" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="3" t="s">
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+    </row>
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B47" s="1" t="s">
         <v>1068</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C47" s="2" t="s">
         <v>1069</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G47" s="3" t="s">
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="48" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="3" t="s">
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+    </row>
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="1" t="s">
         <v>1070</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="C48" s="2" t="s">
         <v>1071</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G48" s="3" t="s">
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="49" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="3" t="s">
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+    </row>
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B49" s="1" t="s">
         <v>1072</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C49" s="2" t="s">
         <v>1073</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G49" s="3" t="s">
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="50" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="3" t="s">
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+    </row>
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B50" s="1" t="s">
         <v>1074</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="C50" s="2" t="s">
         <v>1075</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G50" s="3" t="s">
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="51" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="3" t="s">
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+    </row>
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
         <v>1026</v>
       </c>
-      <c r="B51" s="3" t="n">
+      <c r="B51" s="1" t="n">
         <v>4610</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C51" s="2" t="s">
         <v>1076</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G51" s="3" t="s">
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="52" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="3" t="s">
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+    </row>
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B52" s="1" t="s">
         <v>1077</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="C52" s="2" t="s">
         <v>1078</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G52" s="3" t="s">
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="53" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="3" t="s">
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+    </row>
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B53" s="1" t="s">
         <v>1079</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="C53" s="2" t="s">
         <v>1080</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G53" s="3" t="s">
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="54" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="3" t="s">
+      <c r="H53" s="2"/>
+      <c r="I53" s="2"/>
+    </row>
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B54" s="1" t="s">
         <v>1081</v>
       </c>
-      <c r="C54" s="3" t="s">
+      <c r="C54" s="2" t="s">
         <v>1082</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G54" s="3" t="s">
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="2" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="55" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="3" t="s">
+      <c r="H54" s="2"/>
+      <c r="I54" s="2"/>
+    </row>
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B55" s="1" t="s">
         <v>1083</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="C55" s="2" t="s">
         <v>1084</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G55" s="3" t="s">
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+      <c r="G55" s="2" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="56" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="3" t="s">
+      <c r="H55" s="2"/>
+      <c r="I55" s="2"/>
+    </row>
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B56" s="1" t="s">
         <v>1085</v>
       </c>
-      <c r="C56" s="3" t="s">
+      <c r="C56" s="2" t="s">
         <v>1086</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G56" s="3" t="s">
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="57" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="3" t="s">
+      <c r="H56" s="2"/>
+      <c r="I56" s="2"/>
+    </row>
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B57" s="1" t="s">
         <v>1087</v>
       </c>
-      <c r="C57" s="3" t="s">
+      <c r="C57" s="2" t="s">
         <v>1088</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G57" s="3" t="s">
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="2" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="58" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="3" t="s">
+      <c r="H57" s="2"/>
+      <c r="I57" s="2"/>
+    </row>
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B58" s="1" t="s">
         <v>1089</v>
       </c>
-      <c r="C58" s="3" t="s">
+      <c r="C58" s="2" t="s">
         <v>1090</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G58" s="3" t="s">
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+      <c r="G58" s="2" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="59" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="3" t="s">
+      <c r="H58" s="2"/>
+      <c r="I58" s="2"/>
+    </row>
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="B59" s="1" t="s">
         <v>1091</v>
       </c>
-      <c r="C59" s="3" t="s">
+      <c r="C59" s="2" t="s">
         <v>1092</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G59" s="3" t="s">
+      <c r="E59" s="2"/>
+      <c r="F59" s="2"/>
+      <c r="G59" s="2" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="60" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="3" t="s">
+      <c r="H59" s="2"/>
+      <c r="I59" s="2"/>
+    </row>
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="s">
         <v>1026</v>
       </c>
-      <c r="B60" s="3" t="n">
+      <c r="B60" s="1" t="n">
         <v>51795710</v>
       </c>
-      <c r="C60" s="3" t="s">
+      <c r="C60" s="2" t="s">
         <v>1093</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G60" s="3" t="s">
+      <c r="E60" s="2"/>
+      <c r="F60" s="2"/>
+      <c r="G60" s="2" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="61" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="3" t="s">
+      <c r="H60" s="2"/>
+      <c r="I60" s="2"/>
+    </row>
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="B61" s="1" t="s">
         <v>1094</v>
       </c>
-      <c r="C61" s="3" t="s">
+      <c r="C61" s="2" t="s">
         <v>1095</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G61" s="3" t="s">
+      <c r="E61" s="2"/>
+      <c r="F61" s="2"/>
+      <c r="G61" s="2" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="62" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="3" t="s">
+      <c r="H61" s="2"/>
+      <c r="I61" s="2"/>
+    </row>
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A62" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="B62" s="1" t="s">
         <v>1096</v>
       </c>
-      <c r="C62" s="3" t="s">
+      <c r="C62" s="2" t="s">
         <v>1097</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G62" s="3" t="s">
+      <c r="E62" s="2"/>
+      <c r="F62" s="2"/>
+      <c r="G62" s="2" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="63" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="3" t="s">
+      <c r="H62" s="2"/>
+      <c r="I62" s="2"/>
+    </row>
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A63" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B63" s="1" t="s">
         <v>1098</v>
       </c>
-      <c r="C63" s="3" t="s">
+      <c r="C63" s="2" t="s">
         <v>1099</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G63" s="3" t="s">
+      <c r="E63" s="2"/>
+      <c r="F63" s="2"/>
+      <c r="G63" s="2" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="64" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="3" t="s">
+      <c r="H63" s="2"/>
+      <c r="I63" s="2"/>
+    </row>
+    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A64" s="1" t="s">
         <v>1026</v>
       </c>
-      <c r="B64" s="3" t="n">
+      <c r="B64" s="1" t="n">
         <v>8198360</v>
       </c>
-      <c r="C64" s="3" t="s">
+      <c r="C64" s="2" t="s">
         <v>1100</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G64" s="3" t="s">
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
+      <c r="G64" s="2" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="65" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="3" t="s">
+      <c r="H64" s="2"/>
+      <c r="I64" s="2"/>
+    </row>
+    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A65" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B65" s="3" t="s">
+      <c r="B65" s="1" t="s">
         <v>1101</v>
       </c>
-      <c r="C65" s="3" t="s">
+      <c r="C65" s="2" t="s">
         <v>1102</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G65" s="3" t="s">
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+      <c r="G65" s="2" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="66" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="3" t="s">
+      <c r="H65" s="2"/>
+      <c r="I65" s="2"/>
+    </row>
+    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A66" s="1" t="s">
         <v>1026</v>
       </c>
-      <c r="B66" s="3" t="n">
+      <c r="B66" s="1" t="n">
         <v>10242166</v>
       </c>
-      <c r="C66" s="3" t="s">
+      <c r="C66" s="2" t="s">
         <v>1103</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G66" s="3" t="s">
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
+      <c r="G66" s="2" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="67" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="3" t="s">
+      <c r="H66" s="2"/>
+      <c r="I66" s="2"/>
+    </row>
+    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A67" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B67" s="3" t="s">
+      <c r="B67" s="1" t="s">
         <v>1104</v>
       </c>
-      <c r="C67" s="3" t="s">
+      <c r="C67" s="2" t="s">
         <v>1105</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G67" s="3" t="s">
+      <c r="E67" s="2"/>
+      <c r="F67" s="2"/>
+      <c r="G67" s="2" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="68" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="3" t="s">
+      <c r="H67" s="2"/>
+      <c r="I67" s="2"/>
+    </row>
+    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A68" s="1" t="s">
         <v>1026</v>
       </c>
-      <c r="B68" s="3" t="n">
+      <c r="B68" s="1" t="n">
         <v>10233351</v>
       </c>
-      <c r="C68" s="3" t="s">
+      <c r="C68" s="2" t="s">
         <v>1106</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G68" s="3" t="s">
+      <c r="E68" s="2"/>
+      <c r="F68" s="2"/>
+      <c r="G68" s="2" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="69" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="3" t="s">
+      <c r="H68" s="2"/>
+      <c r="I68" s="2"/>
+    </row>
+    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A69" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B69" s="3" t="s">
+      <c r="B69" s="1" t="s">
         <v>1107</v>
       </c>
-      <c r="C69" s="3" t="s">
+      <c r="C69" s="2" t="s">
         <v>1108</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G69" s="3" t="s">
+      <c r="E69" s="2"/>
+      <c r="F69" s="2"/>
+      <c r="G69" s="2" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="70" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="3" t="s">
+      <c r="H69" s="2"/>
+      <c r="I69" s="2"/>
+    </row>
+    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A70" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B70" s="3" t="s">
+      <c r="B70" s="1" t="s">
         <v>1109</v>
       </c>
-      <c r="C70" s="3" t="s">
+      <c r="C70" s="2" t="s">
         <v>1110</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G70" s="3" t="s">
+      <c r="E70" s="2"/>
+      <c r="F70" s="2"/>
+      <c r="G70" s="2" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="71" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="3" t="s">
+      <c r="H70" s="2"/>
+      <c r="I70" s="2"/>
+    </row>
+    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A71" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B71" s="3" t="s">
+      <c r="B71" s="1" t="s">
         <v>1111</v>
       </c>
-      <c r="C71" s="3" t="s">
+      <c r="C71" s="2" t="s">
         <v>1112</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G71" s="3" t="s">
+      <c r="E71" s="2"/>
+      <c r="F71" s="2"/>
+      <c r="G71" s="2" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="72" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="3" t="s">
+      <c r="H71" s="2"/>
+      <c r="I71" s="2"/>
+    </row>
+    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A72" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B72" s="3" t="s">
+      <c r="B72" s="1" t="s">
         <v>1113</v>
       </c>
-      <c r="C72" s="3" t="s">
+      <c r="C72" s="2" t="s">
         <v>1114</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G72" s="3" t="s">
+      <c r="E72" s="2"/>
+      <c r="F72" s="2"/>
+      <c r="G72" s="2" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="73" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="3" t="s">
+      <c r="H72" s="2"/>
+      <c r="I72" s="2"/>
+    </row>
+    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A73" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="B73" s="1" t="s">
         <v>1115</v>
       </c>
-      <c r="C73" s="3" t="s">
+      <c r="C73" s="2" t="s">
         <v>1116</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G73" s="3" t="s">
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
+      <c r="G73" s="2" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="74" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="3" t="s">
+      <c r="H73" s="2"/>
+      <c r="I73" s="2"/>
+    </row>
+    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A74" s="1" t="s">
         <v>1026</v>
       </c>
-      <c r="B74" s="3" t="n">
+      <c r="B74" s="1" t="n">
         <v>8189514</v>
       </c>
-      <c r="C74" s="3" t="s">
+      <c r="C74" s="2" t="s">
         <v>1117</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G74" s="3" t="s">
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
+      <c r="G74" s="2" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="75" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="3" t="s">
+      <c r="H74" s="2"/>
+      <c r="I74" s="2"/>
+    </row>
+    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A75" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="B75" s="1" t="s">
         <v>1118</v>
       </c>
-      <c r="C75" s="3" t="s">
+      <c r="C75" s="2" t="s">
         <v>1119</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G75" s="3" t="s">
+      <c r="E75" s="2"/>
+      <c r="F75" s="2"/>
+      <c r="G75" s="2" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="76" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="3" t="s">
+      <c r="H75" s="2"/>
+      <c r="I75" s="2"/>
+    </row>
+    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A76" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B76" s="3" t="s">
+      <c r="B76" s="1" t="s">
         <v>1120</v>
       </c>
-      <c r="C76" s="3" t="s">
+      <c r="C76" s="2" t="s">
         <v>1121</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G76" s="3" t="s">
+      <c r="E76" s="2"/>
+      <c r="F76" s="2"/>
+      <c r="G76" s="2" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="77" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="3" t="s">
+      <c r="H76" s="2"/>
+      <c r="I76" s="2"/>
+    </row>
+    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A77" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B77" s="3" t="s">
+      <c r="B77" s="1" t="s">
         <v>1122</v>
       </c>
-      <c r="C77" s="3" t="s">
+      <c r="C77" s="2" t="s">
         <v>1123</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G77" s="3" t="s">
+      <c r="E77" s="2"/>
+      <c r="F77" s="2"/>
+      <c r="G77" s="2" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="78" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="3" t="s">
+      <c r="H77" s="2"/>
+      <c r="I77" s="2"/>
+    </row>
+    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A78" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B78" s="3" t="s">
+      <c r="B78" s="1" t="s">
         <v>1124</v>
       </c>
-      <c r="C78" s="3" t="s">
+      <c r="C78" s="2" t="s">
         <v>1125</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G78" s="3" t="s">
+      <c r="E78" s="2"/>
+      <c r="F78" s="2"/>
+      <c r="G78" s="2" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="79" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="3" t="s">
+      <c r="H78" s="2"/>
+      <c r="I78" s="2"/>
+    </row>
+    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A79" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B79" s="3" t="s">
+      <c r="B79" s="1" t="s">
         <v>1126</v>
       </c>
-      <c r="C79" s="3" t="s">
+      <c r="C79" s="2" t="s">
         <v>1127</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G79" s="3" t="s">
+      <c r="E79" s="2"/>
+      <c r="F79" s="2"/>
+      <c r="G79" s="2" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="80" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="3" t="s">
+      <c r="H79" s="2"/>
+      <c r="I79" s="2"/>
+    </row>
+    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A80" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B80" s="3" t="s">
+      <c r="B80" s="1" t="s">
         <v>1128</v>
       </c>
-      <c r="C80" s="3" t="s">
+      <c r="C80" s="2" t="s">
         <v>1129</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G80" s="3" t="s">
+      <c r="E80" s="2"/>
+      <c r="F80" s="2"/>
+      <c r="G80" s="2" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="81" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="3" t="s">
+      <c r="H80" s="2"/>
+      <c r="I80" s="2"/>
+    </row>
+    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A81" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B81" s="3" t="s">
+      <c r="B81" s="1" t="s">
         <v>1130</v>
       </c>
-      <c r="C81" s="3" t="s">
+      <c r="C81" s="2" t="s">
         <v>1131</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G81" s="3" t="s">
+      <c r="E81" s="2"/>
+      <c r="F81" s="2"/>
+      <c r="G81" s="2" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="82" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="3" t="s">
+      <c r="H81" s="2"/>
+      <c r="I81" s="2"/>
+    </row>
+    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A82" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B82" s="3" t="s">
+      <c r="B82" s="1" t="s">
         <v>1132</v>
       </c>
-      <c r="C82" s="3" t="s">
+      <c r="C82" s="2" t="s">
         <v>1133</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G82" s="3" t="s">
+      <c r="E82" s="2"/>
+      <c r="F82" s="2"/>
+      <c r="G82" s="2" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="83" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="3" t="s">
+      <c r="H82" s="2"/>
+      <c r="I82" s="2"/>
+    </row>
+    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A83" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B83" s="3" t="s">
+      <c r="B83" s="1" t="s">
         <v>1134</v>
       </c>
-      <c r="C83" s="3" t="s">
+      <c r="C83" s="2" t="s">
         <v>1135</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G83" s="3" t="s">
+      <c r="E83" s="2"/>
+      <c r="F83" s="2"/>
+      <c r="G83" s="2" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="84" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="3" t="s">
+      <c r="H83" s="2"/>
+      <c r="I83" s="2"/>
+    </row>
+    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A84" s="1" t="s">
         <v>1026</v>
       </c>
-      <c r="B84" s="3" t="n">
+      <c r="B84" s="1" t="n">
         <v>10246126</v>
       </c>
-      <c r="C84" s="3" t="s">
+      <c r="C84" s="2" t="s">
         <v>1136</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G84" s="3" t="s">
+      <c r="E84" s="2"/>
+      <c r="F84" s="2"/>
+      <c r="G84" s="2" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="85" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="3" t="s">
+      <c r="H84" s="2"/>
+      <c r="I84" s="2"/>
+    </row>
+    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A85" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B85" s="3" t="s">
+      <c r="B85" s="1" t="s">
         <v>1137</v>
       </c>
-      <c r="C85" s="3" t="s">
+      <c r="C85" s="2" t="s">
         <v>1138</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G85" s="3" t="s">
+      <c r="E85" s="2"/>
+      <c r="F85" s="2"/>
+      <c r="G85" s="2" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="86" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="3" t="s">
+      <c r="H85" s="2"/>
+      <c r="I85" s="2"/>
+    </row>
+    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A86" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B86" s="3" t="s">
+      <c r="B86" s="1" t="s">
         <v>1139</v>
       </c>
-      <c r="C86" s="3" t="s">
+      <c r="C86" s="2" t="s">
         <v>1140</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G86" s="3" t="s">
+      <c r="E86" s="2"/>
+      <c r="F86" s="2"/>
+      <c r="G86" s="2" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="87" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="3" t="s">
+      <c r="H86" s="2"/>
+      <c r="I86" s="2"/>
+    </row>
+    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A87" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B87" s="3" t="s">
+      <c r="B87" s="1" t="s">
         <v>1141</v>
       </c>
-      <c r="C87" s="3" t="s">
+      <c r="C87" s="2" t="s">
         <v>1142</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G87" s="3" t="s">
+      <c r="E87" s="2"/>
+      <c r="F87" s="2"/>
+      <c r="G87" s="2" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="88" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="3" t="s">
+      <c r="H87" s="2"/>
+      <c r="I87" s="2"/>
+    </row>
+    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A88" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B88" s="3" t="s">
+      <c r="B88" s="1" t="s">
         <v>1143</v>
       </c>
-      <c r="C88" s="3" t="s">
+      <c r="C88" s="2" t="s">
         <v>1144</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G88" s="3" t="s">
+      <c r="E88" s="2"/>
+      <c r="F88" s="2"/>
+      <c r="G88" s="2" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="89" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="3" t="s">
+      <c r="H88" s="2"/>
+      <c r="I88" s="2"/>
+    </row>
+    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A89" s="1" t="s">
         <v>1026</v>
       </c>
-      <c r="B89" s="3" t="n">
+      <c r="B89" s="1" t="n">
         <v>8888253</v>
       </c>
-      <c r="C89" s="3" t="s">
+      <c r="C89" s="2" t="s">
         <v>1145</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G89" s="3" t="s">
+      <c r="E89" s="2"/>
+      <c r="F89" s="2"/>
+      <c r="G89" s="2" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="90" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="3" t="s">
+      <c r="H89" s="2"/>
+      <c r="I89" s="2"/>
+    </row>
+    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A90" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B90" s="3" t="s">
+      <c r="B90" s="1" t="s">
         <v>1146</v>
       </c>
-      <c r="C90" s="3" t="s">
+      <c r="C90" s="2" t="s">
         <v>1147</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G90" s="3" t="s">
+      <c r="E90" s="2"/>
+      <c r="F90" s="2"/>
+      <c r="G90" s="2" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="91" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="3" t="s">
+      <c r="H90" s="2"/>
+      <c r="I90" s="2"/>
+    </row>
+    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A91" s="1" t="s">
         <v>1026</v>
       </c>
-      <c r="B91" s="3" t="n">
+      <c r="B91" s="1" t="n">
         <v>8546048</v>
       </c>
-      <c r="C91" s="3" t="s">
+      <c r="C91" s="2" t="s">
         <v>1148</v>
       </c>
       <c r="D91" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G91" s="3" t="s">
+      <c r="E91" s="2"/>
+      <c r="F91" s="2"/>
+      <c r="G91" s="2" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="92" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="3" t="s">
+      <c r="H91" s="2"/>
+      <c r="I91" s="2"/>
+    </row>
+    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A92" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B92" s="3" t="s">
+      <c r="B92" s="1" t="s">
         <v>1149</v>
       </c>
-      <c r="C92" s="3" t="s">
+      <c r="C92" s="2" t="s">
         <v>1150</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G92" s="3" t="s">
+      <c r="E92" s="2"/>
+      <c r="F92" s="2"/>
+      <c r="G92" s="2" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="93" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="3" t="s">
+      <c r="H92" s="2"/>
+      <c r="I92" s="2"/>
+    </row>
+    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A93" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B93" s="3" t="s">
+      <c r="B93" s="1" t="s">
         <v>1151</v>
       </c>
-      <c r="C93" s="3" t="s">
+      <c r="C93" s="2" t="s">
         <v>1152</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G93" s="3" t="s">
+      <c r="E93" s="2"/>
+      <c r="F93" s="2"/>
+      <c r="G93" s="2" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="94" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="3" t="s">
+      <c r="H93" s="2"/>
+      <c r="I93" s="2"/>
+    </row>
+    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A94" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B94" s="3" t="s">
+      <c r="B94" s="1" t="s">
         <v>1153</v>
       </c>
-      <c r="C94" s="3" t="s">
+      <c r="C94" s="2" t="s">
         <v>1154</v>
       </c>
       <c r="D94" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G94" s="3" t="s">
+      <c r="E94" s="2"/>
+      <c r="F94" s="2"/>
+      <c r="G94" s="2" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="95" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="3" t="s">
+      <c r="H94" s="2"/>
+      <c r="I94" s="2"/>
+    </row>
+    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A95" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B95" s="3" t="s">
+      <c r="B95" s="1" t="s">
         <v>1155</v>
       </c>
-      <c r="C95" s="3" t="s">
+      <c r="C95" s="2" t="s">
         <v>1156</v>
       </c>
       <c r="D95" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G95" s="3" t="s">
+      <c r="E95" s="2"/>
+      <c r="F95" s="2"/>
+      <c r="G95" s="2" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="96" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="3" t="s">
+      <c r="H95" s="2"/>
+      <c r="I95" s="2"/>
+    </row>
+    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A96" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B96" s="3" t="s">
+      <c r="B96" s="1" t="s">
         <v>1157</v>
       </c>
-      <c r="C96" s="3" t="s">
+      <c r="C96" s="2" t="s">
         <v>1158</v>
       </c>
       <c r="D96" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G96" s="3" t="s">
+      <c r="E96" s="2"/>
+      <c r="F96" s="2"/>
+      <c r="G96" s="2" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="97" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="3" t="s">
+      <c r="H96" s="2"/>
+      <c r="I96" s="2"/>
+    </row>
+    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A97" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B97" s="3" t="s">
+      <c r="B97" s="1" t="s">
         <v>1159</v>
       </c>
-      <c r="C97" s="3" t="s">
+      <c r="C97" s="2" t="s">
         <v>1160</v>
       </c>
       <c r="D97" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G97" s="3" t="s">
+      <c r="E97" s="2"/>
+      <c r="F97" s="2"/>
+      <c r="G97" s="2" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="98" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="3" t="s">
+      <c r="H97" s="2"/>
+      <c r="I97" s="2"/>
+    </row>
+    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A98" s="1" t="s">
         <v>1026</v>
       </c>
-      <c r="B98" s="3" t="n">
+      <c r="B98" s="1" t="n">
         <v>10285797</v>
       </c>
-      <c r="C98" s="3" t="s">
+      <c r="C98" s="2" t="s">
         <v>1161</v>
       </c>
       <c r="D98" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G98" s="3" t="s">
+      <c r="E98" s="2"/>
+      <c r="F98" s="2"/>
+      <c r="G98" s="2" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="99" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="3" t="s">
+      <c r="H98" s="2"/>
+      <c r="I98" s="2"/>
+    </row>
+    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A99" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="B99" s="3" t="s">
+      <c r="B99" s="1" t="s">
         <v>1162</v>
       </c>
-      <c r="C99" s="3" t="s">
+      <c r="C99" s="2" t="s">
         <v>1163</v>
       </c>
       <c r="D99" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G99" s="3" t="s">
+      <c r="E99" s="2"/>
+      <c r="F99" s="2"/>
+      <c r="G99" s="2" t="s">
         <v>355</v>
       </c>
+      <c r="H99" s="2"/>
+      <c r="I99" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:I99"/>
@@ -6793,13 +7132,13 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B11" activeCellId="1" sqref="E27:E29 B11"/>
+      <selection pane="topRight" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="3" width="10.8178137651822"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="27.6356275303644"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="28.0647773279352"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="3" width="10.8178137651822"/>
   </cols>
   <sheetData>
@@ -6872,16 +7211,16 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" activeCellId="1" sqref="E27:E29 B2"/>
+      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="3" width="10.8178137651822"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="3" width="10.8178137651822"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="16.9230769230769"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="3" width="27.8502024291498"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="3" width="28.2793522267206"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="3" width="10.8178137651822"/>
   </cols>
   <sheetData>
@@ -7054,18 +7393,18 @@
   </sheetPr>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
-      <selection pane="bottomRight" activeCell="D6" activeCellId="1" sqref="E27:E29 D6"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="3" width="10.8178137651822"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="23.4574898785425"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="3" width="10.8178137651822"/>
   </cols>
   <sheetData>
@@ -7150,20 +7489,20 @@
   <dimension ref="A1:J108"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="L53" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B86" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="L1" activeCellId="0" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="A53" activeCellId="0" sqref="A53"/>
-      <selection pane="bottomRight" activeCell="C57" activeCellId="1" sqref="E27:E29 C57"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A86" activeCellId="0" sqref="A86"/>
+      <selection pane="bottomRight" activeCell="B108" activeCellId="0" sqref="B108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="3" width="10.8178137651822"/>
     <col collapsed="false" hidden="false" max="4" min="3" style="6" width="10.8178137651822"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="15.9595141700405"/>
     <col collapsed="false" hidden="false" max="9" min="6" style="3" width="10.8178137651822"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="3" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="3" width="23.8866396761134"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="3" width="10.8178137651822"/>
   </cols>
   <sheetData>
@@ -9505,203 +9844,369 @@
       </c>
       <c r="I84" s="9"/>
     </row>
-    <row r="85" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="3" t="s">
+    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A85" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="B85" s="3" t="s">
+      <c r="B85" s="8" t="s">
         <v>357</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H85" s="3" t="s">
+      <c r="D85" s="8"/>
+      <c r="E85" s="9"/>
+      <c r="F85" s="9"/>
+      <c r="G85" s="9"/>
+      <c r="H85" s="9" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="3" t="s">
+      <c r="I85" s="9"/>
+    </row>
+    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A86" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="H86" s="3" t="s">
+      <c r="B86" s="8"/>
+      <c r="C86" s="2"/>
+      <c r="D86" s="8"/>
+      <c r="E86" s="9"/>
+      <c r="F86" s="9"/>
+      <c r="G86" s="9"/>
+      <c r="H86" s="9" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="3" t="s">
+      <c r="I86" s="9"/>
+    </row>
+    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A87" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="H87" s="3" t="s">
+      <c r="B87" s="8"/>
+      <c r="C87" s="2"/>
+      <c r="D87" s="8"/>
+      <c r="E87" s="9"/>
+      <c r="F87" s="9"/>
+      <c r="G87" s="9"/>
+      <c r="H87" s="9" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="3" t="s">
+      <c r="I87" s="9"/>
+    </row>
+    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A88" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="H88" s="3" t="s">
+      <c r="B88" s="8"/>
+      <c r="C88" s="2"/>
+      <c r="D88" s="8"/>
+      <c r="E88" s="9"/>
+      <c r="F88" s="9"/>
+      <c r="G88" s="9"/>
+      <c r="H88" s="9" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="3" t="s">
+      <c r="I88" s="9"/>
+    </row>
+    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A89" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="H89" s="3" t="s">
+      <c r="B89" s="8"/>
+      <c r="C89" s="2"/>
+      <c r="D89" s="8"/>
+      <c r="E89" s="9"/>
+      <c r="F89" s="9"/>
+      <c r="G89" s="9"/>
+      <c r="H89" s="9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="3" t="s">
+      <c r="I89" s="9"/>
+    </row>
+    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A90" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="H90" s="3" t="s">
+      <c r="B90" s="8"/>
+      <c r="C90" s="2"/>
+      <c r="D90" s="8"/>
+      <c r="E90" s="9"/>
+      <c r="F90" s="9"/>
+      <c r="G90" s="9"/>
+      <c r="H90" s="9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="3" t="s">
+      <c r="I90" s="9"/>
+    </row>
+    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A91" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="H91" s="3" t="s">
+      <c r="B91" s="8"/>
+      <c r="C91" s="2"/>
+      <c r="D91" s="8"/>
+      <c r="E91" s="9"/>
+      <c r="F91" s="9"/>
+      <c r="G91" s="9"/>
+      <c r="H91" s="9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="3" t="s">
+      <c r="I91" s="9"/>
+    </row>
+    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A92" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="H92" s="3" t="s">
+      <c r="B92" s="8"/>
+      <c r="C92" s="2"/>
+      <c r="D92" s="8"/>
+      <c r="E92" s="9"/>
+      <c r="F92" s="9"/>
+      <c r="G92" s="9"/>
+      <c r="H92" s="9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="3" t="s">
+      <c r="I92" s="9"/>
+    </row>
+    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A93" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="H93" s="3" t="s">
+      <c r="B93" s="8"/>
+      <c r="C93" s="2"/>
+      <c r="D93" s="8"/>
+      <c r="E93" s="9"/>
+      <c r="F93" s="9"/>
+      <c r="G93" s="9"/>
+      <c r="H93" s="9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="3" t="s">
+      <c r="I93" s="9"/>
+    </row>
+    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A94" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="H94" s="3" t="s">
+      <c r="B94" s="8"/>
+      <c r="C94" s="2"/>
+      <c r="D94" s="8"/>
+      <c r="E94" s="9"/>
+      <c r="F94" s="9"/>
+      <c r="G94" s="9"/>
+      <c r="H94" s="9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="3" t="s">
+      <c r="I94" s="9"/>
+    </row>
+    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A95" s="1" t="s">
         <v>369</v>
       </c>
-      <c r="H95" s="3" t="s">
+      <c r="B95" s="8"/>
+      <c r="C95" s="2"/>
+      <c r="D95" s="8"/>
+      <c r="E95" s="9"/>
+      <c r="F95" s="9"/>
+      <c r="G95" s="9"/>
+      <c r="H95" s="9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="3" t="s">
+      <c r="I95" s="9"/>
+    </row>
+    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A96" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="H96" s="3" t="s">
+      <c r="B96" s="8"/>
+      <c r="C96" s="2"/>
+      <c r="D96" s="8"/>
+      <c r="E96" s="9"/>
+      <c r="F96" s="9"/>
+      <c r="G96" s="9"/>
+      <c r="H96" s="9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="3" t="s">
+      <c r="I96" s="9"/>
+    </row>
+    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A97" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="H97" s="3" t="s">
+      <c r="B97" s="8"/>
+      <c r="C97" s="2"/>
+      <c r="D97" s="8"/>
+      <c r="E97" s="9"/>
+      <c r="F97" s="9"/>
+      <c r="G97" s="9"/>
+      <c r="H97" s="9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="3" t="s">
+      <c r="I97" s="9"/>
+    </row>
+    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A98" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="H98" s="3" t="s">
+      <c r="B98" s="8"/>
+      <c r="C98" s="2"/>
+      <c r="D98" s="8"/>
+      <c r="E98" s="9"/>
+      <c r="F98" s="9"/>
+      <c r="G98" s="9"/>
+      <c r="H98" s="9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="3" t="s">
+      <c r="I98" s="9"/>
+    </row>
+    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A99" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="H99" s="3" t="s">
+      <c r="B99" s="8"/>
+      <c r="C99" s="2"/>
+      <c r="D99" s="8"/>
+      <c r="E99" s="9"/>
+      <c r="F99" s="9"/>
+      <c r="G99" s="9"/>
+      <c r="H99" s="9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="3" t="s">
+      <c r="I99" s="9"/>
+    </row>
+    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A100" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="H100" s="3" t="s">
+      <c r="B100" s="8"/>
+      <c r="C100" s="2"/>
+      <c r="D100" s="8"/>
+      <c r="E100" s="9"/>
+      <c r="F100" s="9"/>
+      <c r="G100" s="9"/>
+      <c r="H100" s="9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="3" t="s">
+      <c r="I100" s="9"/>
+    </row>
+    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A101" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="H101" s="3" t="s">
+      <c r="B101" s="8"/>
+      <c r="C101" s="2"/>
+      <c r="D101" s="8"/>
+      <c r="E101" s="9"/>
+      <c r="F101" s="9"/>
+      <c r="G101" s="9"/>
+      <c r="H101" s="9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="3" t="s">
+      <c r="I101" s="9"/>
+    </row>
+    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A102" s="1" t="s">
         <v>376</v>
       </c>
-      <c r="H102" s="3" t="s">
+      <c r="B102" s="8"/>
+      <c r="C102" s="2"/>
+      <c r="D102" s="8"/>
+      <c r="E102" s="9"/>
+      <c r="F102" s="9"/>
+      <c r="G102" s="9"/>
+      <c r="H102" s="9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="3" t="s">
+      <c r="I102" s="9"/>
+    </row>
+    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A103" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="H103" s="3" t="s">
+      <c r="B103" s="8"/>
+      <c r="C103" s="2"/>
+      <c r="D103" s="8"/>
+      <c r="E103" s="9"/>
+      <c r="F103" s="9"/>
+      <c r="G103" s="9"/>
+      <c r="H103" s="9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="3" t="s">
+      <c r="I103" s="9"/>
+    </row>
+    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A104" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="H104" s="3" t="s">
+      <c r="B104" s="8"/>
+      <c r="C104" s="2"/>
+      <c r="D104" s="8"/>
+      <c r="E104" s="9"/>
+      <c r="F104" s="9"/>
+      <c r="G104" s="9"/>
+      <c r="H104" s="9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="3" t="s">
+      <c r="I104" s="9"/>
+    </row>
+    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A105" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="H105" s="3" t="s">
+      <c r="B105" s="8"/>
+      <c r="C105" s="2"/>
+      <c r="D105" s="8"/>
+      <c r="E105" s="9"/>
+      <c r="F105" s="9"/>
+      <c r="G105" s="9"/>
+      <c r="H105" s="9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="3" t="s">
+      <c r="I105" s="9"/>
+    </row>
+    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A106" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="H106" s="3" t="s">
+      <c r="B106" s="8"/>
+      <c r="C106" s="2"/>
+      <c r="D106" s="8"/>
+      <c r="E106" s="9"/>
+      <c r="F106" s="9"/>
+      <c r="G106" s="9"/>
+      <c r="H106" s="9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="3" t="s">
+      <c r="I106" s="9"/>
+    </row>
+    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A107" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="H107" s="3" t="s">
+      <c r="B107" s="8"/>
+      <c r="C107" s="2"/>
+      <c r="D107" s="8"/>
+      <c r="E107" s="9"/>
+      <c r="F107" s="9"/>
+      <c r="G107" s="9"/>
+      <c r="H107" s="9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="3" t="s">
+      <c r="I107" s="9"/>
+    </row>
+    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A108" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="H108" s="3" t="s">
+      <c r="B108" s="8"/>
+      <c r="C108" s="2"/>
+      <c r="D108" s="8"/>
+      <c r="E108" s="9"/>
+      <c r="F108" s="9"/>
+      <c r="G108" s="9"/>
+      <c r="H108" s="9" t="s">
         <v>27</v>
       </c>
+      <c r="I108" s="9"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J84"/>
@@ -9728,7 +10233,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A56" activeCellId="0" sqref="A56"/>
-      <selection pane="bottomRight" activeCell="F62" activeCellId="1" sqref="E27:E29 F62"/>
+      <selection pane="bottomRight" activeCell="A62" activeCellId="0" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -10112,6 +10617,7 @@
       <c r="B34" s="13" t="n">
         <v>0.0005</v>
       </c>
+      <c r="C34" s="0"/>
       <c r="D34" s="14"/>
     </row>
     <row r="35" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10133,6 +10639,7 @@
       <c r="B36" s="13" t="n">
         <v>0.0005</v>
       </c>
+      <c r="C36" s="0"/>
       <c r="D36" s="14"/>
     </row>
     <row r="37" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10154,6 +10661,7 @@
       <c r="B38" s="13" t="n">
         <v>0.0005</v>
       </c>
+      <c r="C38" s="0"/>
       <c r="D38" s="14"/>
     </row>
     <row r="39" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10175,6 +10683,7 @@
       <c r="B40" s="13" t="n">
         <v>0.0005</v>
       </c>
+      <c r="C40" s="0"/>
       <c r="D40" s="14"/>
     </row>
     <row r="41" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10196,6 +10705,7 @@
       <c r="B42" s="13" t="n">
         <v>0.0005</v>
       </c>
+      <c r="C42" s="0"/>
       <c r="D42" s="14"/>
     </row>
     <row r="43" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10241,6 +10751,7 @@
       <c r="B46" s="13" t="n">
         <v>0.0005</v>
       </c>
+      <c r="C46" s="0"/>
       <c r="D46" s="14"/>
     </row>
     <row r="47" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10485,20 +10996,20 @@
   </sheetPr>
   <dimension ref="A1:I87"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
-      <selection pane="bottomRight" activeCell="D6" activeCellId="1" sqref="E27:E29 D6"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B62" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A62" activeCellId="0" sqref="A62"/>
+      <selection pane="bottomRight" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="23.1376518218623"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="23.995951417004"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="24.4251012145749"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="3" width="10.8178137651822"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="33.4210526315789"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="34.0647773279352"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="3" width="10.8178137651822"/>
   </cols>
   <sheetData>
@@ -10544,11 +11055,13 @@
       <c r="D2" s="2" t="s">
         <v>457</v>
       </c>
-      <c r="E2" s="16" t="b">
+      <c r="E2" s="16" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
+      <c r="H2" s="0"/>
       <c r="I2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10564,11 +11077,13 @@
       <c r="D3" s="2" t="s">
         <v>460</v>
       </c>
-      <c r="E3" s="16" t="b">
+      <c r="E3" s="16" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
+      <c r="H3" s="0"/>
       <c r="I3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10584,11 +11099,13 @@
       <c r="D4" s="2" t="s">
         <v>463</v>
       </c>
-      <c r="E4" s="16" t="b">
+      <c r="E4" s="16" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
+      <c r="H4" s="0"/>
       <c r="I4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10604,11 +11121,13 @@
       <c r="D5" s="2" t="s">
         <v>466</v>
       </c>
-      <c r="E5" s="16" t="b">
+      <c r="E5" s="16" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
+      <c r="H5" s="0"/>
       <c r="I5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10624,11 +11143,13 @@
       <c r="D6" s="2" t="s">
         <v>469</v>
       </c>
-      <c r="E6" s="16" t="b">
+      <c r="E6" s="16" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
+      <c r="H6" s="0"/>
       <c r="I6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10644,11 +11165,13 @@
       <c r="D7" s="2" t="s">
         <v>472</v>
       </c>
-      <c r="E7" s="16" t="b">
+      <c r="E7" s="16" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
+      <c r="H7" s="0"/>
       <c r="I7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10664,11 +11187,13 @@
       <c r="D8" s="2" t="s">
         <v>475</v>
       </c>
-      <c r="E8" s="16" t="b">
+      <c r="E8" s="16" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
+      <c r="H8" s="0"/>
       <c r="I8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10684,11 +11209,13 @@
       <c r="D9" s="2" t="s">
         <v>478</v>
       </c>
-      <c r="E9" s="16" t="b">
+      <c r="E9" s="16" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
+      <c r="H9" s="0"/>
       <c r="I9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10704,11 +11231,13 @@
       <c r="D10" s="2" t="s">
         <v>481</v>
       </c>
-      <c r="E10" s="16" t="b">
+      <c r="E10" s="16" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
+      <c r="H10" s="0"/>
       <c r="I10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10724,11 +11253,13 @@
       <c r="D11" s="2" t="s">
         <v>484</v>
       </c>
-      <c r="E11" s="16" t="b">
+      <c r="E11" s="16" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
+      <c r="H11" s="0"/>
       <c r="I11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10744,11 +11275,13 @@
       <c r="D12" s="2" t="s">
         <v>487</v>
       </c>
-      <c r="E12" s="16" t="b">
+      <c r="E12" s="16" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
+      <c r="H12" s="0"/>
       <c r="I12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10764,11 +11297,13 @@
       <c r="D13" s="2" t="s">
         <v>490</v>
       </c>
-      <c r="E13" s="16" t="b">
+      <c r="E13" s="16" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
+      <c r="H13" s="0"/>
       <c r="I13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10784,11 +11319,13 @@
       <c r="D14" s="2" t="s">
         <v>493</v>
       </c>
-      <c r="E14" s="16" t="b">
+      <c r="E14" s="16" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
+      <c r="H14" s="0"/>
       <c r="I14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10804,11 +11341,13 @@
       <c r="D15" s="2" t="s">
         <v>496</v>
       </c>
-      <c r="E15" s="16" t="b">
+      <c r="E15" s="16" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
+      <c r="H15" s="0"/>
       <c r="I15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10824,11 +11363,13 @@
       <c r="D16" s="2" t="s">
         <v>499</v>
       </c>
-      <c r="E16" s="16" t="b">
+      <c r="E16" s="16" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
+      <c r="H16" s="0"/>
       <c r="I16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10844,11 +11385,13 @@
       <c r="D17" s="2" t="s">
         <v>502</v>
       </c>
-      <c r="E17" s="16" t="b">
+      <c r="E17" s="16" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
+      <c r="H17" s="0"/>
       <c r="I17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10864,11 +11407,13 @@
       <c r="D18" s="2" t="s">
         <v>505</v>
       </c>
-      <c r="E18" s="16" t="b">
+      <c r="E18" s="16" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
+      <c r="H18" s="0"/>
       <c r="I18" s="2"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10884,11 +11429,13 @@
       <c r="D19" s="2" t="s">
         <v>508</v>
       </c>
-      <c r="E19" s="16" t="b">
+      <c r="E19" s="16" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
+      <c r="H19" s="0"/>
       <c r="I19" s="2"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10904,11 +11451,13 @@
       <c r="D20" s="2" t="s">
         <v>511</v>
       </c>
-      <c r="E20" s="16" t="b">
+      <c r="E20" s="16" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
+      <c r="H20" s="0"/>
       <c r="I20" s="2"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10924,11 +11473,13 @@
       <c r="D21" s="2" t="s">
         <v>514</v>
       </c>
-      <c r="E21" s="16" t="b">
+      <c r="E21" s="16" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
+      <c r="H21" s="0"/>
       <c r="I21" s="2"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10944,11 +11495,13 @@
       <c r="D22" s="2" t="s">
         <v>517</v>
       </c>
-      <c r="E22" s="16" t="b">
+      <c r="E22" s="16" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
+      <c r="H22" s="0"/>
       <c r="I22" s="2"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10964,11 +11517,13 @@
       <c r="D23" s="2" t="s">
         <v>520</v>
       </c>
-      <c r="E23" s="16" t="b">
+      <c r="E23" s="16" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
+      <c r="H23" s="0"/>
       <c r="I23" s="2"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10984,11 +11539,13 @@
       <c r="D24" s="2" t="s">
         <v>523</v>
       </c>
-      <c r="E24" s="16" t="b">
+      <c r="E24" s="16" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
+      <c r="H24" s="0"/>
       <c r="I24" s="2"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11004,11 +11561,13 @@
       <c r="D25" s="2" t="s">
         <v>526</v>
       </c>
-      <c r="E25" s="16" t="b">
+      <c r="E25" s="16" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
+      <c r="H25" s="0"/>
       <c r="I25" s="2"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11024,11 +11583,13 @@
       <c r="D26" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="E26" s="16" t="b">
+      <c r="E26" s="16" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
+      <c r="H26" s="0"/>
       <c r="I26" s="2"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11044,11 +11605,13 @@
       <c r="D27" s="2" t="s">
         <v>532</v>
       </c>
-      <c r="E27" s="16" t="b">
+      <c r="E27" s="16" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
+      <c r="H27" s="0"/>
       <c r="I27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11064,11 +11627,13 @@
       <c r="D28" s="2" t="s">
         <v>535</v>
       </c>
-      <c r="E28" s="16" t="b">
+      <c r="E28" s="16" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
+      <c r="H28" s="0"/>
       <c r="I28" s="2"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11084,11 +11649,13 @@
       <c r="D29" s="2" t="s">
         <v>538</v>
       </c>
-      <c r="E29" s="16" t="b">
+      <c r="E29" s="16" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
+      <c r="H29" s="0"/>
       <c r="I29" s="2"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11104,11 +11671,13 @@
       <c r="D30" s="2" t="s">
         <v>541</v>
       </c>
-      <c r="E30" s="16" t="b">
+      <c r="E30" s="16" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
+      <c r="H30" s="0"/>
       <c r="I30" s="2"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11124,11 +11693,13 @@
       <c r="D31" s="2" t="s">
         <v>544</v>
       </c>
-      <c r="E31" s="16" t="b">
+      <c r="E31" s="16" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
+      <c r="H31" s="0"/>
       <c r="I31" s="2"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11144,11 +11715,13 @@
       <c r="D32" s="2" t="s">
         <v>547</v>
       </c>
-      <c r="E32" s="16" t="b">
+      <c r="E32" s="16" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
+      <c r="H32" s="0"/>
       <c r="I32" s="2"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11164,11 +11737,13 @@
       <c r="D33" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="E33" s="16" t="b">
+      <c r="E33" s="16" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
+      <c r="H33" s="0"/>
       <c r="I33" s="2"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11184,11 +11759,13 @@
       <c r="D34" s="2" t="s">
         <v>553</v>
       </c>
-      <c r="E34" s="16" t="b">
+      <c r="E34" s="16" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
+      <c r="H34" s="0"/>
       <c r="I34" s="2"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11204,11 +11781,13 @@
       <c r="D35" s="2" t="s">
         <v>556</v>
       </c>
-      <c r="E35" s="16" t="b">
+      <c r="E35" s="16" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
+      <c r="H35" s="0"/>
       <c r="I35" s="2"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11224,11 +11803,13 @@
       <c r="D36" s="2" t="s">
         <v>559</v>
       </c>
-      <c r="E36" s="16" t="b">
+      <c r="E36" s="16" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
+      <c r="H36" s="0"/>
       <c r="I36" s="2"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11244,11 +11825,13 @@
       <c r="D37" s="2" t="s">
         <v>562</v>
       </c>
-      <c r="E37" s="16" t="b">
+      <c r="E37" s="16" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
+      <c r="H37" s="0"/>
       <c r="I37" s="2"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11264,11 +11847,13 @@
       <c r="D38" s="2" t="s">
         <v>565</v>
       </c>
-      <c r="E38" s="16" t="b">
+      <c r="E38" s="16" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
+      <c r="H38" s="0"/>
       <c r="I38" s="2"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11284,11 +11869,13 @@
       <c r="D39" s="2" t="s">
         <v>568</v>
       </c>
-      <c r="E39" s="16" t="b">
+      <c r="E39" s="16" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
+      <c r="H39" s="0"/>
       <c r="I39" s="2"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11304,11 +11891,13 @@
       <c r="D40" s="2" t="s">
         <v>571</v>
       </c>
-      <c r="E40" s="16" t="b">
+      <c r="E40" s="16" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
+      <c r="H40" s="0"/>
       <c r="I40" s="2"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11324,11 +11913,13 @@
       <c r="D41" s="2" t="s">
         <v>574</v>
       </c>
-      <c r="E41" s="16" t="b">
+      <c r="E41" s="16" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
+      <c r="H41" s="0"/>
       <c r="I41" s="2"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11344,11 +11935,13 @@
       <c r="D42" s="2" t="s">
         <v>577</v>
       </c>
-      <c r="E42" s="16" t="b">
+      <c r="E42" s="16" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
+      <c r="H42" s="0"/>
       <c r="I42" s="2"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11364,11 +11957,13 @@
       <c r="D43" s="2" t="s">
         <v>580</v>
       </c>
-      <c r="E43" s="16" t="b">
+      <c r="E43" s="16" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
+      <c r="H43" s="0"/>
       <c r="I43" s="2"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11384,11 +11979,13 @@
       <c r="D44" s="2" t="s">
         <v>583</v>
       </c>
-      <c r="E44" s="16" t="b">
+      <c r="E44" s="16" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
+      <c r="H44" s="0"/>
       <c r="I44" s="2"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11404,11 +12001,13 @@
       <c r="D45" s="2" t="s">
         <v>586</v>
       </c>
-      <c r="E45" s="16" t="b">
+      <c r="E45" s="16" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
+      <c r="H45" s="0"/>
       <c r="I45" s="2"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11424,11 +12023,13 @@
       <c r="D46" s="2" t="s">
         <v>589</v>
       </c>
-      <c r="E46" s="16" t="b">
+      <c r="E46" s="16" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
+      <c r="H46" s="0"/>
       <c r="I46" s="2"/>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11444,11 +12045,13 @@
       <c r="D47" s="2" t="s">
         <v>592</v>
       </c>
-      <c r="E47" s="16" t="b">
+      <c r="E47" s="16" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
+      <c r="H47" s="0"/>
       <c r="I47" s="2"/>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11464,11 +12067,13 @@
       <c r="D48" s="2" t="s">
         <v>595</v>
       </c>
-      <c r="E48" s="16" t="b">
+      <c r="E48" s="16" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
+      <c r="H48" s="0"/>
       <c r="I48" s="2"/>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11484,11 +12089,13 @@
       <c r="D49" s="2" t="s">
         <v>598</v>
       </c>
-      <c r="E49" s="16" t="b">
+      <c r="E49" s="16" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
+      <c r="H49" s="0"/>
       <c r="I49" s="2"/>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11504,11 +12111,13 @@
       <c r="D50" s="2" t="s">
         <v>601</v>
       </c>
-      <c r="E50" s="16" t="b">
+      <c r="E50" s="16" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
+      <c r="H50" s="0"/>
       <c r="I50" s="2"/>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11524,11 +12133,13 @@
       <c r="D51" s="2" t="s">
         <v>604</v>
       </c>
-      <c r="E51" s="16" t="b">
+      <c r="E51" s="16" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
+      <c r="H51" s="0"/>
       <c r="I51" s="2"/>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11544,11 +12155,13 @@
       <c r="D52" s="2" t="s">
         <v>607</v>
       </c>
-      <c r="E52" s="16" t="b">
+      <c r="E52" s="16" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
+      <c r="H52" s="0"/>
       <c r="I52" s="2"/>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11564,11 +12177,13 @@
       <c r="D53" s="2" t="s">
         <v>610</v>
       </c>
-      <c r="E53" s="16" t="b">
+      <c r="E53" s="16" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
+      <c r="H53" s="0"/>
       <c r="I53" s="2"/>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11584,11 +12199,13 @@
       <c r="D54" s="2" t="s">
         <v>613</v>
       </c>
-      <c r="E54" s="16" t="b">
+      <c r="E54" s="16" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
+      <c r="H54" s="0"/>
       <c r="I54" s="2"/>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11604,11 +12221,13 @@
       <c r="D55" s="2" t="s">
         <v>616</v>
       </c>
-      <c r="E55" s="16" t="b">
+      <c r="E55" s="16" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="F55" s="2"/>
       <c r="G55" s="2"/>
+      <c r="H55" s="0"/>
       <c r="I55" s="2"/>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11624,11 +12243,13 @@
       <c r="D56" s="2" t="s">
         <v>619</v>
       </c>
-      <c r="E56" s="16" t="b">
+      <c r="E56" s="16" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F56" s="2"/>
       <c r="G56" s="2"/>
+      <c r="H56" s="0"/>
       <c r="I56" s="2"/>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11644,11 +12265,13 @@
       <c r="D57" s="2" t="s">
         <v>622</v>
       </c>
-      <c r="E57" s="16" t="b">
+      <c r="E57" s="16" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
+      <c r="H57" s="0"/>
       <c r="I57" s="2"/>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11664,11 +12287,13 @@
       <c r="D58" s="2" t="s">
         <v>625</v>
       </c>
-      <c r="E58" s="16" t="b">
+      <c r="E58" s="16" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F58" s="2"/>
       <c r="G58" s="2"/>
+      <c r="H58" s="0"/>
       <c r="I58" s="2"/>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11684,11 +12309,13 @@
       <c r="D59" s="2" t="s">
         <v>628</v>
       </c>
-      <c r="E59" s="16" t="b">
+      <c r="E59" s="16" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="F59" s="2"/>
       <c r="G59" s="2"/>
+      <c r="H59" s="0"/>
       <c r="I59" s="2"/>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11704,11 +12331,13 @@
       <c r="D60" s="2" t="s">
         <v>631</v>
       </c>
-      <c r="E60" s="16" t="b">
+      <c r="E60" s="16" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="F60" s="2"/>
       <c r="G60" s="2"/>
+      <c r="H60" s="0"/>
       <c r="I60" s="2"/>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11724,11 +12353,13 @@
       <c r="D61" s="2" t="s">
         <v>634</v>
       </c>
-      <c r="E61" s="16" t="b">
+      <c r="E61" s="16" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="F61" s="2"/>
       <c r="G61" s="2"/>
+      <c r="H61" s="0"/>
       <c r="I61" s="2"/>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11744,11 +12375,13 @@
       <c r="D62" s="2" t="s">
         <v>637</v>
       </c>
-      <c r="E62" s="16" t="b">
+      <c r="E62" s="16" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F62" s="2"/>
       <c r="G62" s="2"/>
+      <c r="H62" s="0"/>
       <c r="I62" s="2"/>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11764,11 +12397,13 @@
       <c r="D63" s="2" t="s">
         <v>640</v>
       </c>
-      <c r="E63" s="16" t="b">
+      <c r="E63" s="16" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F63" s="2"/>
       <c r="G63" s="2"/>
+      <c r="H63" s="0"/>
       <c r="I63" s="2"/>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11784,11 +12419,13 @@
       <c r="D64" s="2" t="s">
         <v>643</v>
       </c>
-      <c r="E64" s="16" t="b">
+      <c r="E64" s="16" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
+      <c r="H64" s="0"/>
       <c r="I64" s="2"/>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11804,11 +12441,13 @@
       <c r="D65" s="2" t="s">
         <v>646</v>
       </c>
-      <c r="E65" s="16" t="b">
+      <c r="E65" s="16" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F65" s="2"/>
       <c r="G65" s="2"/>
+      <c r="H65" s="0"/>
       <c r="I65" s="2"/>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11824,11 +12463,13 @@
       <c r="D66" s="2" t="s">
         <v>649</v>
       </c>
-      <c r="E66" s="16" t="b">
+      <c r="E66" s="16" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F66" s="2"/>
       <c r="G66" s="2"/>
+      <c r="H66" s="0"/>
       <c r="I66" s="2"/>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11844,11 +12485,13 @@
       <c r="D67" s="2" t="s">
         <v>652</v>
       </c>
-      <c r="E67" s="16" t="b">
+      <c r="E67" s="16" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F67" s="2"/>
       <c r="G67" s="2"/>
+      <c r="H67" s="0"/>
       <c r="I67" s="2"/>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11864,11 +12507,13 @@
       <c r="D68" s="2" t="s">
         <v>655</v>
       </c>
-      <c r="E68" s="16" t="b">
+      <c r="E68" s="16" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F68" s="2"/>
       <c r="G68" s="2"/>
+      <c r="H68" s="0"/>
       <c r="I68" s="2"/>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11884,11 +12529,13 @@
       <c r="D69" s="2" t="s">
         <v>658</v>
       </c>
-      <c r="E69" s="16" t="b">
+      <c r="E69" s="16" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F69" s="2"/>
       <c r="G69" s="2"/>
+      <c r="H69" s="0"/>
       <c r="I69" s="2"/>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11904,11 +12551,13 @@
       <c r="D70" s="2" t="s">
         <v>661</v>
       </c>
-      <c r="E70" s="16" t="b">
+      <c r="E70" s="16" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F70" s="2"/>
       <c r="G70" s="2"/>
+      <c r="H70" s="0"/>
       <c r="I70" s="2"/>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11924,11 +12573,13 @@
       <c r="D71" s="2" t="s">
         <v>664</v>
       </c>
-      <c r="E71" s="16" t="b">
+      <c r="E71" s="16" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="F71" s="2"/>
       <c r="G71" s="2"/>
+      <c r="H71" s="0"/>
       <c r="I71" s="2"/>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11944,11 +12595,13 @@
       <c r="D72" s="2" t="s">
         <v>667</v>
       </c>
-      <c r="E72" s="16" t="b">
+      <c r="E72" s="16" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="F72" s="2"/>
       <c r="G72" s="2"/>
+      <c r="H72" s="0"/>
       <c r="I72" s="2"/>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11964,11 +12617,13 @@
       <c r="D73" s="2" t="s">
         <v>670</v>
       </c>
-      <c r="E73" s="16" t="b">
+      <c r="E73" s="16" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F73" s="2"/>
       <c r="G73" s="2"/>
+      <c r="H73" s="0"/>
       <c r="I73" s="2"/>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11984,11 +12639,13 @@
       <c r="D74" s="2" t="s">
         <v>673</v>
       </c>
-      <c r="E74" s="16" t="b">
+      <c r="E74" s="16" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="F74" s="2"/>
       <c r="G74" s="2"/>
+      <c r="H74" s="0"/>
       <c r="I74" s="2"/>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12004,11 +12661,13 @@
       <c r="D75" s="2" t="s">
         <v>676</v>
       </c>
-      <c r="E75" s="16" t="b">
+      <c r="E75" s="16" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F75" s="2"/>
       <c r="G75" s="2"/>
+      <c r="H75" s="0"/>
       <c r="I75" s="2"/>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12024,11 +12683,13 @@
       <c r="D76" s="2" t="s">
         <v>679</v>
       </c>
-      <c r="E76" s="16" t="b">
+      <c r="E76" s="16" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="F76" s="2"/>
       <c r="G76" s="2"/>
+      <c r="H76" s="0"/>
       <c r="I76" s="2"/>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12044,11 +12705,13 @@
       <c r="D77" s="2" t="s">
         <v>682</v>
       </c>
-      <c r="E77" s="16" t="b">
+      <c r="E77" s="16" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="F77" s="2"/>
       <c r="G77" s="2"/>
+      <c r="H77" s="0"/>
       <c r="I77" s="2"/>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12064,11 +12727,13 @@
       <c r="D78" s="2" t="s">
         <v>685</v>
       </c>
-      <c r="E78" s="16" t="b">
+      <c r="E78" s="16" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="F78" s="2"/>
       <c r="G78" s="2"/>
+      <c r="H78" s="0"/>
       <c r="I78" s="2"/>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12084,11 +12749,13 @@
       <c r="D79" s="2" t="s">
         <v>688</v>
       </c>
-      <c r="E79" s="16" t="b">
+      <c r="E79" s="16" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F79" s="2"/>
       <c r="G79" s="2"/>
+      <c r="H79" s="0"/>
       <c r="I79" s="2"/>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12104,11 +12771,13 @@
       <c r="D80" s="2" t="s">
         <v>691</v>
       </c>
-      <c r="E80" s="16" t="b">
+      <c r="E80" s="16" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F80" s="2"/>
       <c r="G80" s="2"/>
+      <c r="H80" s="0"/>
       <c r="I80" s="2"/>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12124,11 +12793,13 @@
       <c r="D81" s="2" t="s">
         <v>694</v>
       </c>
-      <c r="E81" s="16" t="b">
+      <c r="E81" s="16" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F81" s="2"/>
       <c r="G81" s="2"/>
+      <c r="H81" s="0"/>
       <c r="I81" s="2"/>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12144,11 +12815,13 @@
       <c r="D82" s="2" t="s">
         <v>697</v>
       </c>
-      <c r="E82" s="16" t="b">
+      <c r="E82" s="16" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F82" s="2"/>
       <c r="G82" s="2"/>
+      <c r="H82" s="0"/>
       <c r="I82" s="2"/>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12164,11 +12837,13 @@
       <c r="D83" s="2" t="s">
         <v>700</v>
       </c>
-      <c r="E83" s="16" t="b">
+      <c r="E83" s="16" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="F83" s="2"/>
       <c r="G83" s="2"/>
+      <c r="H83" s="0"/>
       <c r="I83" s="2"/>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12184,11 +12859,13 @@
       <c r="D84" s="2" t="s">
         <v>703</v>
       </c>
-      <c r="E84" s="16" t="b">
+      <c r="E84" s="16" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="F84" s="2"/>
       <c r="G84" s="2"/>
+      <c r="H84" s="0"/>
       <c r="I84" s="2"/>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12204,11 +12881,13 @@
       <c r="D85" s="2" t="s">
         <v>706</v>
       </c>
-      <c r="E85" s="16" t="b">
+      <c r="E85" s="16" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="F85" s="2"/>
       <c r="G85" s="2"/>
+      <c r="H85" s="0"/>
       <c r="I85" s="2"/>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12224,7 +12903,8 @@
       <c r="D86" s="2" t="s">
         <v>709</v>
       </c>
-      <c r="E86" s="16" t="b">
+      <c r="E86" s="16" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F86" s="2"/>
@@ -12245,7 +12925,8 @@
       <c r="D87" s="2" t="s">
         <v>712</v>
       </c>
-      <c r="E87" s="16" t="b">
+      <c r="E87" s="16" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F87" s="2"/>
@@ -12273,19 +12954,19 @@
   </sheetPr>
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
-      <selection pane="bottomRight" activeCell="E27" activeCellId="0" sqref="E27:E29"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="D27" activeCellId="0" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="18.9595141700405"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="3" width="10.8178137651822"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="22.2793522267206"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="22.6032388663968"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="3" width="10.8178137651822"/>
   </cols>
   <sheetData>
@@ -12913,22 +13594,22 @@
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
-      <selection pane="bottomRight" activeCell="E34" activeCellId="1" sqref="E27:E29 E34"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="E34" activeCellId="0" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="18" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="18" width="17.1376518218624"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="18" width="20.4615384615385"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="18" width="10.2834008097166"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="18" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="18" width="17.3522267206478"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="18" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="18" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="18" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="18" width="21.2105263157895"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="18" width="16.1740890688259"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="18" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="18" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="18" width="10.8178137651822"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
start to standardize database identifiers
</commit_message>
<xml_diff>
--- a/random_wc_model_generator/data/fixtures/model_core.xlsx
+++ b/random_wc_model_generator/data/fixtures/model_core.xlsx
@@ -41,7 +41,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Submodels!$A$1:$I$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Taxon!$A$1:$B$6</definedName>
   </definedNames>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -4958,10 +4958,21 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="U28" sqref="U28"/>
+      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42" customWidth="1"/>
+    <col min="3" max="3" width="56.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">

</xml_diff>